<commit_message>
Added MPXC2011DT1 to sensor list.
</commit_message>
<xml_diff>
--- a/Sensor Cluster Team/ElectricalReqMat.xlsx
+++ b/Sensor Cluster Team/ElectricalReqMat.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AQaut\Documents\OffsetVentilator\Sensor Cluster Team\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\OffsetVentilator\Sensor Cluster Team\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188DA4C1-1E97-4FD6-A48D-D26E349EF859}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sensors" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="115">
   <si>
     <t>USER INTERACE</t>
   </si>
@@ -370,11 +369,33 @@
   <si>
     <t>https://www.digikey.com/product-detail/en/murata-electronics/PKM22EPPH4012-B0/490-7032-ND/2595278</t>
   </si>
+  <si>
+    <t>MPXC2011TD1</t>
+  </si>
+  <si>
+    <t>SIL4</t>
+  </si>
+  <si>
+    <t>https://www.findchips.com/search/mpxc2011dt1</t>
+  </si>
+  <si>
+    <t>Range: 0-100 hPa</t>
+  </si>
+  <si>
+    <t>Differential Analog</t>
+  </si>
+  <si>
+    <t>Approved for medical (vents in particular)
+Temperature Compensated</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -460,7 +481,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -500,12 +521,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -522,6 +537,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -803,45 +827,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:K29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:K30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22:J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.77734375" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" customWidth="1"/>
-    <col min="5" max="5" width="26.88671875" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" customWidth="1"/>
-    <col min="7" max="7" width="26.6640625" customWidth="1"/>
-    <col min="8" max="9" width="21.77734375" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" customWidth="1"/>
+    <col min="8" max="9" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="22" t="s">
         <v>93</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="21" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D5" s="4" t="s">
         <v>1</v>
       </c>
@@ -864,7 +888,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:11" ht="30" x14ac:dyDescent="0.25">
       <c r="D6" s="5" t="s">
         <v>3</v>
       </c>
@@ -887,7 +911,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:11" ht="45" x14ac:dyDescent="0.25">
       <c r="D7" s="5" t="s">
         <v>13</v>
       </c>
@@ -908,7 +932,7 @@
       </c>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="3:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:11" ht="60" x14ac:dyDescent="0.25">
       <c r="D8" s="5" t="s">
         <v>16</v>
       </c>
@@ -931,7 +955,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -939,7 +963,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -947,7 +971,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>28</v>
       </c>
@@ -958,7 +982,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D12" s="10" t="s">
         <v>44</v>
       </c>
@@ -984,7 +1008,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="3:11" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:11" ht="71.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D13" s="5" t="s">
         <v>32</v>
       </c>
@@ -1010,7 +1034,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="3:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D14" s="14" t="s">
         <v>34</v>
       </c>
@@ -1024,7 +1048,7 @@
       <c r="J14" s="12"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="3:11" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:11" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" s="14" t="s">
         <v>35</v>
       </c>
@@ -1044,7 +1068,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="3:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:11" ht="60" x14ac:dyDescent="0.25">
       <c r="D16" s="12" t="s">
         <v>37</v>
       </c>
@@ -1070,7 +1094,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="3:11" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:11" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" s="12" t="s">
         <v>38</v>
       </c>
@@ -1096,7 +1120,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="3:11" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:11" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D18" s="14" t="s">
         <v>39</v>
       </c>
@@ -1114,7 +1138,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="3:11" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:11" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>73</v>
       </c>
@@ -1137,80 +1161,95 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="D21" s="17" t="s">
+    <row r="20" spans="3:11" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="F20" s="26">
+        <v>5.82</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D22" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-    </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-    </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-    </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-    </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-    </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-    </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-    </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C28" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="25"/>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -1218,50 +1257,62 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="3:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="D29" s="2" t="s">
+    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="3:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="D30" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D21:J26"/>
+    <mergeCell ref="D22:J27"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K13" r:id="rId1" xr:uid="{50BD0665-7000-47E2-8DDA-3AA860FF01F1}"/>
-    <hyperlink ref="K15" r:id="rId2" xr:uid="{497BE04E-D5F8-4396-AFE1-F3346093BC92}"/>
+    <hyperlink ref="K13" r:id="rId1"/>
+    <hyperlink ref="K15" r:id="rId2"/>
+    <hyperlink ref="K20" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E137A05-B8E1-477C-BB75-D32BBC321682}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="26.77734375" customWidth="1"/>
-    <col min="5" max="5" width="26.21875" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="43.6640625" customWidth="1"/>
+    <col min="8" max="8" width="43.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D4" s="4" t="s">
         <v>44</v>
       </c>
@@ -1278,17 +1329,17 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="3:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:9" ht="45" x14ac:dyDescent="0.25">
       <c r="D5" s="12" t="s">
         <v>77</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="17">
         <v>9.9499999999999993</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="17" t="s">
         <v>87</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -1298,46 +1349,46 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="3:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:9" ht="60" x14ac:dyDescent="0.25">
       <c r="D6" s="12" t="s">
         <v>81</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="17">
         <v>7.05</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="20" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="3:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:9" ht="60" x14ac:dyDescent="0.25">
       <c r="D7" s="12" t="s">
         <v>83</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="19" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D12" s="4" t="s">
         <v>44</v>
       </c>
@@ -1354,7 +1405,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="3:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:9" ht="45" x14ac:dyDescent="0.25">
       <c r="D13" s="12" t="s">
         <v>101</v>
       </c>
@@ -1372,7 +1423,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D14" s="12" t="s">
         <v>103</v>
       </c>
@@ -1387,14 +1438,14 @@
       </c>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D15" s="25" t="s">
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D15" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="F15" s="24">
+      <c r="F15" s="22">
         <v>0.78</v>
       </c>
       <c r="G15" s="12" t="s">

</xml_diff>